<commit_message>
Se trabaja sobre #8. Se corrije trialsPromediados en OnlineModule.py
</commit_message>
<xml_diff>
--- a/scripts/Bases/tablaMovs.xlsx
+++ b/scripts/Bases/tablaMovs.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reposBCICompetition\BCIC-Personal\scripts\Bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F555F643-FE98-48EB-82E5-73247B53C9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E767FF1A-2070-4D71-9575-85FCB6C44961}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -82,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -510,6 +509,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,7 +537,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,6 +687,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -988,11 +1020,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BD165-4197-4C0B-9C16-A52D10485F2D}">
-  <dimension ref="B1:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,39 +1035,41 @@
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D2" s="42" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="43"/>
       <c r="G2" s="44"/>
-      <c r="H2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="46"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="45" t="s">
+        <v>0</v>
+      </c>
       <c r="J2" s="46"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="39" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="40"/>
       <c r="N2" s="40"/>
-      <c r="O2" s="41"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
     </row>
-    <row r="3" spans="2:15" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="30" t="s">
         <v>1</v>
       </c>
@@ -1048,32 +1082,33 @@
       <c r="G3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="34" t="s">
+      <c r="H3" s="52"/>
+      <c r="I3" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="K3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="L3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="O3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="P3" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="48" t="s">
         <v>12</v>
@@ -1090,32 +1125,35 @@
       <c r="G4" s="16">
         <v>0</v>
       </c>
-      <c r="H4" s="24">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1</v>
+      <c r="H4" s="53">
+        <v>4</v>
+      </c>
+      <c r="I4" s="24">
+        <v>0</v>
       </c>
       <c r="J4" s="6">
         <v>1</v>
       </c>
-      <c r="K4" s="25">
-        <v>1</v>
-      </c>
-      <c r="L4" s="21">
-        <v>0</v>
-      </c>
-      <c r="M4" s="7">
+      <c r="K4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="25">
+        <v>1</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N4" s="7">
-        <v>1</v>
-      </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+      <c r="P4" s="8">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="49"/>
       <c r="D5" s="17">
@@ -1130,32 +1168,35 @@
       <c r="G5" s="18">
         <v>0</v>
       </c>
-      <c r="H5" s="26">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
+      <c r="H5" s="54">
+        <v>2</v>
+      </c>
+      <c r="I5" s="26">
+        <v>1</v>
       </c>
       <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="27">
-        <v>1</v>
-      </c>
-      <c r="L5" s="22">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27">
+        <v>1</v>
+      </c>
+      <c r="M5" s="22">
         <v>1.2</v>
       </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
       <c r="N5" s="4">
         <v>0</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="49"/>
       <c r="D6" s="17">
@@ -1170,32 +1211,35 @@
       <c r="G6" s="18">
         <v>0</v>
       </c>
-      <c r="H6" s="26">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="H6" s="54">
+        <v>0</v>
+      </c>
+      <c r="I6" s="26">
         <v>1</v>
       </c>
       <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="27">
-        <v>1</v>
-      </c>
-      <c r="L6" s="22">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="27">
+        <v>1</v>
+      </c>
+      <c r="M6" s="22">
         <v>1.2</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="10">
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="50"/>
       <c r="D7" s="19">
@@ -1210,32 +1254,35 @@
       <c r="G7" s="20">
         <v>1</v>
       </c>
-      <c r="H7" s="28">
-        <v>1</v>
-      </c>
-      <c r="I7" s="12">
+      <c r="H7" s="55">
+        <v>1</v>
+      </c>
+      <c r="I7" s="28">
         <v>1</v>
       </c>
       <c r="J7" s="12">
         <v>1</v>
       </c>
-      <c r="K7" s="29">
-        <v>0</v>
-      </c>
-      <c r="L7" s="23">
+      <c r="K7" s="12">
+        <v>1</v>
+      </c>
+      <c r="L7" s="29">
+        <v>0</v>
+      </c>
+      <c r="M7" s="23">
         <v>1.2</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N7" s="13">
-        <v>1</v>
-      </c>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
+        <v>1</v>
+      </c>
+      <c r="P7" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" s="48" t="s">
         <v>13</v>
       </c>
@@ -1251,32 +1298,35 @@
       <c r="G8" s="16">
         <v>0</v>
       </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
+      <c r="H8" s="53">
+        <v>6</v>
+      </c>
+      <c r="I8" s="24">
         <v>0</v>
       </c>
       <c r="J8" s="6">
-        <v>1</v>
-      </c>
-      <c r="K8" s="25">
-        <v>1</v>
-      </c>
-      <c r="L8" s="21">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+      <c r="L8" s="25">
+        <v>1</v>
+      </c>
+      <c r="M8" s="21">
         <v>0</v>
       </c>
       <c r="N8" s="7">
         <v>0</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" s="49"/>
       <c r="D9" s="17">
         <v>1</v>
@@ -1290,32 +1340,35 @@
       <c r="G9" s="18">
         <v>1</v>
       </c>
-      <c r="H9" s="26">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1</v>
+      <c r="H9" s="54">
+        <v>5</v>
+      </c>
+      <c r="I9" s="26">
+        <v>0</v>
       </c>
       <c r="J9" s="3">
         <v>1</v>
       </c>
-      <c r="K9" s="27">
-        <v>0</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>1</v>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="27">
+        <v>0</v>
+      </c>
+      <c r="M9" s="22">
+        <v>0</v>
       </c>
       <c r="N9" s="4">
-        <v>0</v>
-      </c>
-      <c r="O9" s="10">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="50"/>
       <c r="D10" s="19">
         <v>0</v>
@@ -1329,37 +1382,40 @@
       <c r="G10" s="20">
         <v>1</v>
       </c>
-      <c r="H10" s="28">
-        <v>1</v>
-      </c>
-      <c r="I10" s="12">
-        <v>0</v>
+      <c r="H10" s="55">
+        <v>3</v>
+      </c>
+      <c r="I10" s="28">
+        <v>1</v>
       </c>
       <c r="J10" s="12">
-        <v>1</v>
-      </c>
-      <c r="K10" s="29">
-        <v>0</v>
-      </c>
-      <c r="L10" s="23">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0</v>
+      </c>
+      <c r="M10" s="23">
         <v>1.2</v>
       </c>
-      <c r="M10" s="13">
-        <v>0</v>
-      </c>
       <c r="N10" s="13">
-        <v>1</v>
-      </c>
-      <c r="O10" s="14">
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <v>1</v>
+      </c>
+      <c r="P10" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1386,9 +1442,9 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="M2:P2"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="I2:L2"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C10"/>
   </mergeCells>

</xml_diff>

<commit_message>
Se cierra #8. Se logra hacer andar en tiempo Online la comunicación ida y vuelta entre los módulos
</commit_message>
<xml_diff>
--- a/scripts/Bases/tablaMovs.xlsx
+++ b/scripts/Bases/tablaMovs.xlsx
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se hacen pruebas online. Todo OK. Se acomoda algoritmo de SVM para clasificar sin usar Banco de filtros
</commit_message>
<xml_diff>
--- a/scripts/Bases/tablaMovs.xlsx
+++ b/scripts/Bases/tablaMovs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reposBCICompetition\BCIC-Personal\scripts\Bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835A7682-C784-46E5-A9EF-798C9A1A6D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,19 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Movimientos posibles</t>
   </si>
@@ -88,12 +82,15 @@
   </si>
   <si>
     <t>b3</t>
+  </si>
+  <si>
+    <t>3 obstaculos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -369,37 +366,71 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -409,66 +440,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -480,7 +455,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,12 +508,81 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,118 +592,52 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -978,106 +956,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1"/>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="56" t="s">
+      <c r="H1" s="34"/>
+      <c r="I1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="34" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3"/>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="51"/>
+      <c r="G3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="50"/>
       <c r="I3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1090,7 +1068,7 @@
       <c r="L3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="52" t="s">
+      <c r="M3" s="31" t="s">
         <v>3</v>
       </c>
       <c r="N3" s="16" t="s">
@@ -1104,64 +1082,64 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="38">
-        <v>0</v>
-      </c>
-      <c r="E4" s="39">
-        <v>0</v>
-      </c>
-      <c r="F4" s="39">
-        <v>0</v>
-      </c>
-      <c r="G4" s="40">
-        <v>1</v>
-      </c>
-      <c r="H4" s="41">
-        <v>1</v>
-      </c>
-      <c r="I4" s="42">
-        <v>1</v>
-      </c>
-      <c r="J4" s="43">
-        <v>1</v>
-      </c>
-      <c r="K4" s="43">
-        <v>1</v>
-      </c>
-      <c r="L4" s="44">
-        <v>0</v>
-      </c>
-      <c r="M4" s="45">
-        <v>1</v>
-      </c>
-      <c r="N4" s="46">
-        <v>1</v>
-      </c>
-      <c r="O4" s="46">
-        <v>1</v>
-      </c>
-      <c r="P4" s="47">
+      <c r="D4" s="51">
+        <v>0</v>
+      </c>
+      <c r="E4" s="52">
+        <v>0</v>
+      </c>
+      <c r="F4" s="52">
+        <v>0</v>
+      </c>
+      <c r="G4" s="53">
+        <v>1</v>
+      </c>
+      <c r="H4" s="54">
+        <v>1</v>
+      </c>
+      <c r="I4" s="55">
+        <v>1</v>
+      </c>
+      <c r="J4" s="56">
+        <v>1</v>
+      </c>
+      <c r="K4" s="56">
+        <v>1</v>
+      </c>
+      <c r="L4" s="57">
+        <v>0</v>
+      </c>
+      <c r="M4" s="58">
+        <v>1</v>
+      </c>
+      <c r="N4" s="59">
+        <v>1</v>
+      </c>
+      <c r="O4" s="59">
+        <v>1</v>
+      </c>
+      <c r="P4" s="60">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="59"/>
-      <c r="D5" s="27">
-        <v>0</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23">
-        <v>1</v>
-      </c>
-      <c r="G5" s="28">
-        <v>0</v>
-      </c>
-      <c r="H5" s="32">
+      <c r="C5" s="47"/>
+      <c r="D5" s="19">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24">
         <v>2</v>
       </c>
       <c r="I5" s="9">
@@ -1176,7 +1154,7 @@
       <c r="L5" s="10">
         <v>1</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="26">
         <v>1</v>
       </c>
       <c r="N5" s="4">
@@ -1189,21 +1167,21 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="59"/>
-      <c r="D6" s="27">
-        <v>0</v>
-      </c>
-      <c r="E6" s="23">
-        <v>1</v>
-      </c>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-      <c r="G6" s="28">
-        <v>0</v>
-      </c>
-      <c r="H6" s="32">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="47"/>
+      <c r="D6" s="19">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
         <v>4</v>
       </c>
       <c r="I6" s="9">
@@ -1218,7 +1196,7 @@
       <c r="L6" s="10">
         <v>1</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="26">
         <v>1</v>
       </c>
       <c r="N6" s="4">
@@ -1231,21 +1209,21 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="60"/>
-      <c r="D7" s="27">
-        <v>1</v>
-      </c>
-      <c r="E7" s="23">
-        <v>0</v>
-      </c>
-      <c r="F7" s="23">
-        <v>0</v>
-      </c>
-      <c r="G7" s="28">
-        <v>0</v>
-      </c>
-      <c r="H7" s="32">
+    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="48"/>
+      <c r="D7" s="19">
+        <v>1</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24">
         <v>8</v>
       </c>
       <c r="I7" s="9">
@@ -1260,7 +1238,7 @@
       <c r="L7" s="10">
         <v>1</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="26">
         <v>0</v>
       </c>
       <c r="N7" s="4">
@@ -1274,22 +1252,22 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="27">
-        <v>0</v>
-      </c>
-      <c r="E8" s="23">
-        <v>0</v>
-      </c>
-      <c r="F8" s="23">
-        <v>1</v>
-      </c>
-      <c r="G8" s="28">
-        <v>1</v>
-      </c>
-      <c r="H8" s="32">
+      <c r="D8" s="19">
+        <v>0</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>1</v>
+      </c>
+      <c r="G8" s="20">
+        <v>1</v>
+      </c>
+      <c r="H8" s="24">
         <v>3</v>
       </c>
       <c r="I8" s="9">
@@ -1304,7 +1282,7 @@
       <c r="L8" s="10">
         <v>0</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="26">
         <v>1</v>
       </c>
       <c r="N8" s="4">
@@ -1318,20 +1296,20 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="59"/>
-      <c r="D9" s="27">
-        <v>0</v>
-      </c>
-      <c r="E9" s="23">
-        <v>1</v>
-      </c>
-      <c r="F9" s="23">
-        <v>0</v>
-      </c>
-      <c r="G9" s="28">
-        <v>1</v>
-      </c>
-      <c r="H9" s="32">
+      <c r="C9" s="47"/>
+      <c r="D9" s="19">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24">
         <v>5</v>
       </c>
       <c r="I9" s="9">
@@ -1346,7 +1324,7 @@
       <c r="L9" s="10">
         <v>0</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="26">
         <v>1</v>
       </c>
       <c r="N9" s="4">
@@ -1360,20 +1338,20 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="60"/>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30">
-        <v>1</v>
-      </c>
-      <c r="F10" s="30">
-        <v>1</v>
-      </c>
-      <c r="G10" s="31">
-        <v>0</v>
-      </c>
-      <c r="H10" s="33">
+      <c r="C10" s="48"/>
+      <c r="D10" s="21">
+        <v>0</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="22">
+        <v>1</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="25">
         <v>6</v>
       </c>
       <c r="I10" s="11">
@@ -1388,7 +1366,7 @@
       <c r="L10" s="12">
         <v>1</v>
       </c>
-      <c r="M10" s="36">
+      <c r="M10" s="27">
         <v>1</v>
       </c>
       <c r="N10" s="7">
@@ -1401,33 +1379,77 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22">
+        <v>1</v>
+      </c>
+      <c r="G11" s="23">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25">
+        <v>7</v>
+      </c>
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" s="27">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>6</v>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>8</v>
+      <c r="C16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se actualiza tabla de probabilidades
</commit_message>
<xml_diff>
--- a/scripts/Bases/tablaMovs.xlsx
+++ b/scripts/Bases/tablaMovs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reposBCICompetition\BCIC-Personal\scripts\Bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835A7682-C784-46E5-A9EF-798C9A1A6D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41A85A-0254-4779-B436-415B3AEF850A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -421,21 +421,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -446,6 +431,69 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -455,7 +503,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,6 +613,36 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,37 +685,46 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -957,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P18"/>
+  <dimension ref="B1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,25 +1108,25 @@
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="37" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="49"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3"/>
@@ -1055,7 +1142,7 @@
       <c r="G3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="50"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1082,51 +1169,51 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="51">
-        <v>0</v>
-      </c>
-      <c r="E4" s="52">
-        <v>0</v>
-      </c>
-      <c r="F4" s="52">
-        <v>0</v>
-      </c>
-      <c r="G4" s="53">
-        <v>1</v>
-      </c>
-      <c r="H4" s="54">
-        <v>1</v>
-      </c>
-      <c r="I4" s="55">
-        <v>1</v>
-      </c>
-      <c r="J4" s="56">
-        <v>1</v>
-      </c>
-      <c r="K4" s="56">
-        <v>1</v>
-      </c>
-      <c r="L4" s="57">
-        <v>0</v>
-      </c>
-      <c r="M4" s="58">
-        <v>1</v>
-      </c>
-      <c r="N4" s="59">
-        <v>1</v>
-      </c>
-      <c r="O4" s="59">
-        <v>1</v>
-      </c>
-      <c r="P4" s="60">
+      <c r="D4" s="37">
+        <v>0</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0</v>
+      </c>
+      <c r="G4" s="39">
+        <v>1</v>
+      </c>
+      <c r="H4" s="40">
+        <v>1</v>
+      </c>
+      <c r="I4" s="41">
+        <v>1</v>
+      </c>
+      <c r="J4" s="42">
+        <v>1</v>
+      </c>
+      <c r="K4" s="42">
+        <v>1</v>
+      </c>
+      <c r="L4" s="43">
+        <v>0</v>
+      </c>
+      <c r="M4" s="44">
+        <v>1</v>
+      </c>
+      <c r="N4" s="45">
+        <v>1</v>
+      </c>
+      <c r="O4" s="45">
+        <v>1</v>
+      </c>
+      <c r="P4" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="47"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="19">
         <v>0</v>
       </c>
@@ -1168,7 +1255,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="47"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="19">
         <v>0</v>
       </c>
@@ -1210,93 +1297,93 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="48"/>
-      <c r="D7" s="19">
-        <v>1</v>
-      </c>
-      <c r="E7" s="18">
-        <v>0</v>
-      </c>
-      <c r="F7" s="18">
-        <v>0</v>
-      </c>
-      <c r="G7" s="20">
-        <v>0</v>
-      </c>
-      <c r="H7" s="24">
+      <c r="C7" s="61"/>
+      <c r="D7" s="62">
+        <v>1</v>
+      </c>
+      <c r="E7" s="63">
+        <v>0</v>
+      </c>
+      <c r="F7" s="63">
+        <v>0</v>
+      </c>
+      <c r="G7" s="64">
+        <v>0</v>
+      </c>
+      <c r="H7" s="65">
         <v>8</v>
       </c>
-      <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
-        <v>1</v>
-      </c>
-      <c r="L7" s="10">
-        <v>1</v>
-      </c>
-      <c r="M7" s="26">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1</v>
-      </c>
-      <c r="O7" s="4">
-        <v>1</v>
-      </c>
-      <c r="P7" s="5">
+      <c r="I7" s="66">
+        <v>0</v>
+      </c>
+      <c r="J7" s="67">
+        <v>1</v>
+      </c>
+      <c r="K7" s="67">
+        <v>1</v>
+      </c>
+      <c r="L7" s="68">
+        <v>1</v>
+      </c>
+      <c r="M7" s="69">
+        <v>0</v>
+      </c>
+      <c r="N7" s="70">
+        <v>1</v>
+      </c>
+      <c r="O7" s="70">
+        <v>1</v>
+      </c>
+      <c r="P7" s="71">
         <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="19">
-        <v>0</v>
-      </c>
-      <c r="E8" s="18">
-        <v>0</v>
-      </c>
-      <c r="F8" s="18">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="24">
+      <c r="D8" s="37">
+        <v>0</v>
+      </c>
+      <c r="E8" s="38">
+        <v>0</v>
+      </c>
+      <c r="F8" s="38">
+        <v>1</v>
+      </c>
+      <c r="G8" s="39">
+        <v>1</v>
+      </c>
+      <c r="H8" s="40">
         <v>3</v>
       </c>
-      <c r="I8" s="9">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0</v>
-      </c>
-      <c r="M8" s="26">
-        <v>1</v>
-      </c>
-      <c r="N8" s="4">
-        <v>1</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5">
+      <c r="I8" s="41">
+        <v>1</v>
+      </c>
+      <c r="J8" s="42">
+        <v>1</v>
+      </c>
+      <c r="K8" s="42">
+        <v>0</v>
+      </c>
+      <c r="L8" s="43">
+        <v>0</v>
+      </c>
+      <c r="M8" s="44">
+        <v>1</v>
+      </c>
+      <c r="N8" s="45">
+        <v>1</v>
+      </c>
+      <c r="O8" s="45">
+        <v>0</v>
+      </c>
+      <c r="P8" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="47"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="19">
         <v>0</v>
       </c>
@@ -1338,7 +1425,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="48"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="21">
         <v>0</v>
       </c>
@@ -1379,82 +1466,209 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="61" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="21">
-        <v>0</v>
-      </c>
-      <c r="E11" s="22">
-        <v>1</v>
-      </c>
-      <c r="F11" s="22">
-        <v>1</v>
-      </c>
-      <c r="G11" s="23">
-        <v>1</v>
-      </c>
-      <c r="H11" s="25">
+      <c r="D11" s="38">
+        <v>0</v>
+      </c>
+      <c r="E11" s="38">
+        <v>1</v>
+      </c>
+      <c r="F11" s="38">
+        <v>1</v>
+      </c>
+      <c r="G11" s="38">
+        <v>1</v>
+      </c>
+      <c r="H11" s="38">
         <v>7</v>
       </c>
-      <c r="I11" s="11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0</v>
-      </c>
-      <c r="M11" s="27">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0</v>
-      </c>
-      <c r="P11" s="8">
+      <c r="I11" s="42">
+        <v>1</v>
+      </c>
+      <c r="J11" s="42">
+        <v>0</v>
+      </c>
+      <c r="K11" s="42">
+        <v>0</v>
+      </c>
+      <c r="L11" s="42">
+        <v>0</v>
+      </c>
+      <c r="M11" s="45">
+        <v>1</v>
+      </c>
+      <c r="N11" s="45">
+        <v>0</v>
+      </c>
+      <c r="O11" s="45">
+        <v>0</v>
+      </c>
+      <c r="P11" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="73"/>
+      <c r="D12" s="18">
+        <v>1</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1</v>
+      </c>
+      <c r="G12" s="18">
+        <v>1</v>
+      </c>
+      <c r="H12" s="18">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>8</v>
+      <c r="C13" s="73"/>
+      <c r="D13" s="18">
+        <v>1</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1</v>
+      </c>
+      <c r="F13" s="18">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <v>1</v>
+      </c>
+      <c r="H13" s="18">
+        <v>13</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="74"/>
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
+      <c r="E14" s="22">
+        <v>1</v>
+      </c>
+      <c r="F14" s="22">
+        <v>1</v>
+      </c>
+      <c r="G14" s="22">
+        <v>0</v>
+      </c>
+      <c r="H14" s="22">
+        <v>14</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C11:C14"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="I2:L2"/>

</xml_diff>